<commit_message>
añadido el lider semanal (Iris) al excel.
</commit_message>
<xml_diff>
--- a/Excel/ASIGNACIONES_SEMANALES.xlsx
+++ b/Excel/ASIGNACIONES_SEMANALES.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\ProyectoFinal_1DAM\ProyectoFinal_1DAM\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD8EE94-5621-4A8D-B718-6010859F1922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,50 +25,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t xml:space="preserve">SEMANA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JACOBO</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="12">
+  <si>
+    <t>SEMANA</t>
+  </si>
+  <si>
+    <t>LIDER</t>
+  </si>
+  <si>
+    <t>JACOBO</t>
   </si>
   <si>
     <t xml:space="preserve">HITO </t>
   </si>
   <si>
-    <t xml:space="preserve">HITO 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAVID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 y 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IRIS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 y 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOAQUIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CARLOS</t>
+    <t>HITO 2</t>
+  </si>
+  <si>
+    <t>DAVID</t>
+  </si>
+  <si>
+    <t>3 y 6</t>
+  </si>
+  <si>
+    <t>IRIS</t>
+  </si>
+  <si>
+    <t>6 y 7</t>
+  </si>
+  <si>
+    <t>JOAQUIN</t>
+  </si>
+  <si>
+    <t>CARLOS</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,22 +76,15 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -104,13 +101,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.4999"/>
+        <fgColor theme="3" tint="0.49989318521683401"/>
         <bgColor rgb="FF3366FF"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -118,69 +115,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -239,60 +194,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0e2841"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e8e8e8"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="e97132"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196b24"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0f9ed5"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="a02b93"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4ea72e"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607d"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -324,7 +295,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -348,7 +319,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -408,101 +379,229 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="235" zoomScaleNormal="235" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75390625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.14"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="n">
+      <c r="B1" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5">
+        <v>4</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6" t="n">
+      <c r="B8" s="5">
         <v>5</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5">
+        <v>5</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="6"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>